<commit_message>
minor chqnges to swarm
</commit_message>
<xml_diff>
--- a/WriteUp/ParamTests/ParameterTests.xlsx
+++ b/WriteUp/ParamTests/ParameterTests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="7965" yWindow="480" windowWidth="19935" windowHeight="12240" activeTab="1"/>
+    <workbookView xWindow="7965" yWindow="480" windowWidth="19935" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="3" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Computers" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Parameters!$A$1:$O$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Parameters!$A$1:$O$58</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -29,7 +29,7 @@
     <author>pablo alvarez</author>
   </authors>
   <commentList>
-    <comment ref="D7" authorId="0">
+    <comment ref="D9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -118,11 +118,13 @@
           </rPr>
           <t xml:space="preserve">EU Commision
 Koc (S-metolachlor) : 110-369, median : 226 l/kg
+IUPAC: 
+Literature value: Kd range 0.33-1.64 mL/g, Koc range 50.0-540 mL/g, soils=33; Other sources: 120.2-309.0 mL/g (R3), Log Koc 2.26 at 25 Deg C (R4)
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="A41" authorId="1">
+    <comment ref="A45" authorId="1">
       <text>
         <r>
           <rPr>
@@ -147,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C42" authorId="0">
+    <comment ref="C46" authorId="0">
       <text>
         <r>
           <rPr>
@@ -167,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="263">
   <si>
     <t xml:space="preserve">epsilon_iso </t>
   </si>
@@ -361,9 +363,6 @@
     <t>Mean water content at 100cm (9.8 kPa) suction pressure for depth z</t>
   </si>
   <si>
-    <t>$ml ^g$</t>
-  </si>
-  <si>
     <t>beta_runoff</t>
   </si>
   <si>
@@ -490,9 +489,6 @@
     <t>140 - 7000</t>
   </si>
   <si>
-    <t>110 - 369</t>
-  </si>
-  <si>
     <t>Adsorption coefficient</t>
   </si>
   <si>
@@ -706,9 +702,6 @@
     <t>Sum of the absolute difference (obs vs sim)</t>
   </si>
   <si>
-    <t>Mass in soil remaining / Tot app mass</t>
-  </si>
-  <si>
     <t>Cum mass export / Tot app mass</t>
   </si>
   <si>
@@ -724,12 +717,6 @@
     <t>Nash</t>
   </si>
   <si>
-    <t>Model Output TSS</t>
-  </si>
-  <si>
-    <t>Total catchment mass in top soil</t>
-  </si>
-  <si>
     <t>Normalized sum sq error</t>
   </si>
   <si>
@@ -754,9 +741,6 @@
     <t>Soils - Delta</t>
   </si>
   <si>
-    <t>Transect &amp; Detailed Masses (heavy &amp; light)</t>
-  </si>
-  <si>
     <t>soil_samples.py</t>
   </si>
   <si>
@@ -772,13 +756,76 @@
     <t>Cum water export</t>
   </si>
   <si>
-    <t>Cum export mass (heavy and light) (a, b)</t>
-  </si>
-  <si>
     <t>Model simulation assumptions, review before GLUE simulations start</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Model tests will then only be run from March 25th to July 12 (110 days)</t>
+    <t>$\theta_{WPz0z1}$</t>
+  </si>
+  <si>
+    <t>0.16 $\pm$ 0.03</t>
+  </si>
+  <si>
+    <t>$\theta_{WPz2}$</t>
+  </si>
+  <si>
+    <t>0.16 (0.13 - 0.19)</t>
+  </si>
+  <si>
+    <t>$\theta_{WPz3+}$</t>
+  </si>
+  <si>
+    <t>Wilting point z &gt; 1200 mm depth</t>
+  </si>
+  <si>
+    <t>Guillaume 2</t>
+  </si>
+  <si>
+    <t>SWARM</t>
+  </si>
+  <si>
+    <t>GLUE</t>
+  </si>
+  <si>
+    <t>Expected hrs</t>
+  </si>
+  <si>
+    <t>Runs</t>
+  </si>
+  <si>
+    <t>Particles</t>
+  </si>
+  <si>
+    <t>Max iterations</t>
+  </si>
+  <si>
+    <t>Days needed</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>Guillaume 1</t>
+  </si>
+  <si>
+    <t>Kd</t>
+  </si>
+  <si>
+    <t>$ml g^{-1}$</t>
+  </si>
+  <si>
+    <t>Freundlich?</t>
+  </si>
+  <si>
+    <t>https://sitem.herts.ac.uk/aeru/iupac/Reports/465.htm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 50 - 540</t>
   </si>
   <si>
     <r>
@@ -793,7 +840,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Oct. 1 2015 to March 25 2016 (177 days)</t>
+      <t>Oct. 1 2015 to March 15 2016 (166 days)</t>
     </r>
     <r>
       <rPr>
@@ -807,22 +854,322 @@
     </r>
   </si>
   <si>
-    <t>$\theta_{WPz0z1}$</t>
-  </si>
-  <si>
-    <t>0.16 $\pm$ 0.03</t>
-  </si>
-  <si>
-    <t>$\theta_{WPz2}$</t>
-  </si>
-  <si>
-    <t>0.16 (0.13 - 0.19)</t>
-  </si>
-  <si>
-    <t>$\theta_{WPz3+}$</t>
-  </si>
-  <si>
-    <t>Wilting point z &gt; 1200 mm depth</t>
+    <t xml:space="preserve"> - Model tests will then only be run from March 15th (JD: 167) to July 12 (JD: 286)    (Tot: 120 days) </t>
+  </si>
+  <si>
+    <t>Illustrations</t>
+  </si>
+  <si>
+    <t>Output Time Series needed</t>
+  </si>
+  <si>
+    <t>m3 / day</t>
+  </si>
+  <si>
+    <t>Catchment hydrology functioning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runoff </t>
+  </si>
+  <si>
+    <t>Lateral flow (combined for all layers)</t>
+  </si>
+  <si>
+    <t>Baseflow (basement layer)</t>
+  </si>
+  <si>
+    <t>Catchment transport</t>
+  </si>
+  <si>
+    <t>ug / day</t>
+  </si>
+  <si>
+    <t>Where in code?</t>
+  </si>
+  <si>
+    <t>Count TSS written</t>
+  </si>
+  <si>
+    <t>Post-processing (Calculate from components)</t>
+  </si>
+  <si>
+    <t>Detailed Masses (heavy &amp; light)</t>
+  </si>
+  <si>
+    <t>Transect Masses (heavy &amp; light)</t>
+  </si>
+  <si>
+    <t>ug</t>
+  </si>
+  <si>
+    <t>16 x 2 = 32</t>
+  </si>
+  <si>
+    <t>Volume discharged</t>
+  </si>
+  <si>
+    <t>Mass outlet (heavy and light)(a, b)</t>
+  </si>
+  <si>
+    <t>Post-processing (Calculate from mass outlet)</t>
+  </si>
+  <si>
+    <t>Runoff mass flux. (heavy &amp; light)</t>
+  </si>
+  <si>
+    <t>Drainage mass flux. (heavy &amp; light)</t>
+  </si>
+  <si>
+    <t>Baseflow mass flux. (heavy &amp; light)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Outlet hydro </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>components</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Outlet pest </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>components</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Soil sink </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>components</t>
+    </r>
+  </si>
+  <si>
+    <t>Degraded</t>
+  </si>
+  <si>
+    <t>Transect (heavy &amp; light)</t>
+  </si>
+  <si>
+    <t>Catchment (heavy &amp; light)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Leached from Top Soil </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(z0 only)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Leached from 30 cm </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(z1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mass in</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> top soil </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>remaining / Tot app mass</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Drainage (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>layer z2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Total catchment mass in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>top soil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (light &amp; heavy)</t>
+    </r>
+  </si>
+  <si>
+    <t>Total catchment mass - Z (heavy &amp; light)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Runoff from Top soil </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(z0)</t>
+    </r>
+  </si>
+  <si>
+    <t>Calculate from outlet components</t>
+  </si>
+  <si>
+    <t>Comments (if any)</t>
+  </si>
+  <si>
+    <t>Aged</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Persistence </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>all depths</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (real = aged + available)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Persistence </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>all depths</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (aged)</t>
+    </r>
+  </si>
+  <si>
+    <t>Real mass</t>
+  </si>
+  <si>
+    <t>Aged mass</t>
   </si>
 </sst>
 </file>
@@ -916,7 +1263,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -959,8 +1306,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1020,8 +1379,125 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1043,8 +1519,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1167,8 +1644,61 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="21" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="22">
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
@@ -1178,6 +1708,7 @@
     <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
@@ -1191,27 +1722,7 @@
     <cellStyle name="Titre 2" xfId="1"/>
     <cellStyle name="Titre 3" xfId="2"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1290,6 +1801,52 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>333375</xdr:colOff>
+          <xdr:row>41</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>914400</xdr:colOff>
+          <xdr:row>53</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3074" name="Object 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3074"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1579,192 +2136,554 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
+    <col min="4" max="4" width="43.42578125" customWidth="1"/>
+    <col min="5" max="5" width="45.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="75" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" s="75" t="s">
+        <v>178</v>
+      </c>
+      <c r="C5" s="75" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="75" t="s">
+        <v>222</v>
+      </c>
+      <c r="E5" s="76"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="76" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="72" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="60" t="s">
+        <v>251</v>
+      </c>
+      <c r="C6" s="60" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" s="61" t="s">
+        <v>253</v>
+      </c>
+      <c r="E6" s="61">
+        <v>2</v>
+      </c>
+      <c r="F6" s="62"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="72"/>
+      <c r="B7" s="61" t="s">
+        <v>261</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" s="61" t="s">
+        <v>254</v>
+      </c>
+      <c r="E7" s="61">
+        <v>2</v>
+      </c>
+      <c r="F7" s="62"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="72"/>
+      <c r="B8" s="61" t="s">
+        <v>262</v>
+      </c>
+      <c r="C8" s="60" t="s">
+        <v>260</v>
+      </c>
+      <c r="D8" s="61" t="s">
+        <v>254</v>
+      </c>
+      <c r="E8" s="61">
+        <v>2</v>
+      </c>
+      <c r="F8" s="62"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="68" t="s">
+        <v>192</v>
+      </c>
+      <c r="B9" s="60" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="60" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" s="61" t="s">
+        <v>238</v>
+      </c>
+      <c r="E9" s="61" t="s">
+        <v>239</v>
+      </c>
+      <c r="F9" s="62"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="68" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" s="60" t="s">
+        <v>194</v>
+      </c>
+      <c r="C10" s="60" t="s">
+        <v>176</v>
+      </c>
+      <c r="D10" s="61" t="s">
+        <v>237</v>
+      </c>
+      <c r="E10" s="61" t="s">
+        <v>232</v>
+      </c>
+      <c r="F10" s="62"/>
+    </row>
+    <row r="12" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="75" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="75"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="68" t="s">
+        <v>185</v>
+      </c>
+      <c r="B13" s="61" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" s="61" t="s">
+        <v>182</v>
+      </c>
+      <c r="D13" s="61" t="s">
         <v>183</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>177</v>
-      </c>
-      <c r="B6" t="s">
-        <v>179</v>
-      </c>
-      <c r="C6" t="s">
-        <v>178</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E13" s="61" t="s">
+        <v>232</v>
+      </c>
+      <c r="F13" s="63" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="68" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>198</v>
-      </c>
-      <c r="B7" t="s">
-        <v>180</v>
-      </c>
-      <c r="C7" t="s">
-        <v>178</v>
-      </c>
-      <c r="D7" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>199</v>
-      </c>
-      <c r="B8" t="s">
-        <v>200</v>
-      </c>
-      <c r="C8" t="s">
-        <v>178</v>
-      </c>
-      <c r="D8" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B14" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="61" t="s">
+        <v>184</v>
+      </c>
+      <c r="E14" s="61">
+        <v>2</v>
+      </c>
+      <c r="F14" s="63"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="67" t="s">
+        <v>187</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" s="52" t="s">
+        <v>184</v>
+      </c>
+      <c r="E15" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="66"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="69" t="s">
+        <v>188</v>
+      </c>
+      <c r="B16" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="D16" s="52" t="s">
+        <v>234</v>
+      </c>
+      <c r="E16" s="52">
+        <v>6</v>
+      </c>
+      <c r="F16" s="66" t="s">
         <v>190</v>
       </c>
-      <c r="B11" t="s">
-        <v>184</v>
-      </c>
-      <c r="C11" t="s">
-        <v>187</v>
-      </c>
-      <c r="D11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>191</v>
-      </c>
-      <c r="B12" t="s">
-        <v>184</v>
-      </c>
-      <c r="C12" t="s">
-        <v>187</v>
-      </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="70"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55" t="s">
+        <v>233</v>
+      </c>
+      <c r="E17" s="55" t="s">
+        <v>236</v>
+      </c>
+      <c r="F17" s="65"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="71" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>192</v>
-      </c>
-      <c r="B13" t="s">
-        <v>184</v>
-      </c>
-      <c r="C13" t="s">
-        <v>187</v>
-      </c>
-      <c r="D13" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>193</v>
-      </c>
-      <c r="B14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C14" t="s">
-        <v>187</v>
-      </c>
-      <c r="D14" t="s">
-        <v>195</v>
-      </c>
-      <c r="E14" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>194</v>
-      </c>
-      <c r="B15" t="s">
-        <v>184</v>
-      </c>
-      <c r="C15" t="s">
-        <v>187</v>
-      </c>
-      <c r="D15" t="s">
-        <v>195</v>
-      </c>
-      <c r="E15" t="s">
-        <v>196</v>
-      </c>
+      <c r="B18" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="D18" s="58" t="s">
+        <v>234</v>
+      </c>
+      <c r="E18" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="64" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="70"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55" t="s">
+        <v>233</v>
+      </c>
+      <c r="E19" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="56"/>
+    </row>
+    <row r="21" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="75" t="s">
+        <v>221</v>
+      </c>
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="75"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="67" t="s">
+        <v>243</v>
+      </c>
+      <c r="B22" s="52" t="s">
+        <v>223</v>
+      </c>
+      <c r="C22" s="51" t="s">
+        <v>224</v>
+      </c>
+      <c r="D22" s="52" t="s">
+        <v>225</v>
+      </c>
+      <c r="E22" s="52">
+        <v>1</v>
+      </c>
+      <c r="F22" s="53"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="73"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="58" t="s">
+        <v>252</v>
+      </c>
+      <c r="E23" s="58">
+        <v>1</v>
+      </c>
+      <c r="F23" s="59"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="73"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="58" t="s">
+        <v>226</v>
+      </c>
+      <c r="E24" s="58">
+        <v>1</v>
+      </c>
+      <c r="F24" s="59"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="74"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="55" t="s">
+        <v>227</v>
+      </c>
+      <c r="E25" s="55">
+        <v>1</v>
+      </c>
+      <c r="F25" s="56"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="67" t="s">
+        <v>244</v>
+      </c>
+      <c r="B26" s="52" t="s">
+        <v>229</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="D26" s="52" t="s">
+        <v>240</v>
+      </c>
+      <c r="E26" s="52">
+        <v>2</v>
+      </c>
+      <c r="F26" s="53"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="73"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="E27" s="58">
+        <v>2</v>
+      </c>
+      <c r="F27" s="59"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="73"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="58" t="s">
+        <v>242</v>
+      </c>
+      <c r="E28" s="58">
+        <v>2</v>
+      </c>
+      <c r="F28" s="59"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="74"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="55" t="s">
+        <v>242</v>
+      </c>
+      <c r="E29" s="55">
+        <v>2</v>
+      </c>
+      <c r="F29" s="56"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="69" t="s">
+        <v>245</v>
+      </c>
+      <c r="B30" s="52" t="s">
+        <v>235</v>
+      </c>
+      <c r="C30" s="51" t="s">
+        <v>246</v>
+      </c>
+      <c r="D30" s="52" t="s">
+        <v>247</v>
+      </c>
+      <c r="E30" s="52">
+        <v>6</v>
+      </c>
+      <c r="F30" s="53"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="70"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="55" t="s">
+        <v>248</v>
+      </c>
+      <c r="E31" s="55">
+        <v>2</v>
+      </c>
+      <c r="F31" s="56"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="69"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="D32" s="52" t="s">
+        <v>248</v>
+      </c>
+      <c r="E32" s="52">
+        <v>2</v>
+      </c>
+      <c r="F32" s="53"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="70"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="56"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="69"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="51" t="s">
+        <v>250</v>
+      </c>
+      <c r="D34" s="52" t="s">
+        <v>248</v>
+      </c>
+      <c r="E34" s="52">
+        <v>2</v>
+      </c>
+      <c r="F34" s="53"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="70"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="56"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="69"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="51" t="s">
+        <v>255</v>
+      </c>
+      <c r="D36" s="52" t="s">
+        <v>248</v>
+      </c>
+      <c r="E36" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="F36" s="53"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="70"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="56"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="69"/>
+      <c r="B38" s="52"/>
+      <c r="C38" s="51" t="s">
+        <v>258</v>
+      </c>
+      <c r="D38" s="52" t="s">
+        <v>248</v>
+      </c>
+      <c r="E38" s="52"/>
+      <c r="F38" s="53"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="70"/>
+      <c r="B39" s="55"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <oleObjects>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Visio.Drawing.15" shapeId="3074" r:id="rId4">
+          <objectPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>333375</xdr:colOff>
+                <xdr:row>41</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>914400</xdr:colOff>
+                <xdr:row>53</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Visio.Drawing.15" shapeId="3074" r:id="rId4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </oleObjects>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1789,13 +2708,13 @@
         <v>31</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>30</v>
@@ -1804,24 +2723,24 @@
         <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -1833,7 +2752,7 @@
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E2" s="25"/>
       <c r="F2" s="26" t="s">
@@ -1843,7 +2762,7 @@
         <v>35</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I2" s="26" t="s">
         <v>42</v>
@@ -1871,7 +2790,7 @@
       </c>
       <c r="C3" s="25"/>
       <c r="D3" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="26" t="s">
@@ -1881,20 +2800,20 @@
         <v>36</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I3" s="26" t="s">
         <v>42</v>
       </c>
       <c r="J3" s="26">
-        <f t="shared" ref="J3:J54" si="0">IF(I3="Yes", 1, 0)</f>
+        <f t="shared" ref="J3:J58" si="0">IF(I3="Yes", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="K3" s="26" t="s">
         <v>42</v>
       </c>
       <c r="L3" s="26">
-        <f t="shared" ref="L3:L54" si="1">IF(K3="Yes", 1, 0)</f>
+        <f t="shared" ref="L3:L58" si="1">IF(K3="Yes", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="N3" s="26"/>
@@ -1909,7 +2828,7 @@
       </c>
       <c r="C4" s="25"/>
       <c r="D4" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E4" s="25"/>
       <c r="F4" s="26" t="s">
@@ -1919,7 +2838,7 @@
         <v>41</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I4" s="26" t="s">
         <v>42</v>
@@ -1947,7 +2866,7 @@
       </c>
       <c r="C5" s="25"/>
       <c r="D5" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E5" s="25"/>
       <c r="F5" s="26" t="s">
@@ -1957,7 +2876,7 @@
         <v>41</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I5" s="26" t="s">
         <v>42</v>
@@ -1985,7 +2904,7 @@
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E6" s="25"/>
       <c r="F6" s="26" t="s">
@@ -1995,7 +2914,7 @@
         <v>38</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I6" s="26" t="s">
         <v>42</v>
@@ -2023,7 +2942,7 @@
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="26" t="s">
@@ -2033,7 +2952,7 @@
         <v>37</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I7" s="26" t="s">
         <v>42</v>
@@ -2060,11 +2979,11 @@
         <v>0.96</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F8" s="26" t="s">
         <v>32</v>
@@ -2073,7 +2992,7 @@
         <v>39</v>
       </c>
       <c r="H8" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I8" s="26" t="s">
         <v>44</v>
@@ -2090,7 +3009,7 @@
         <v>1</v>
       </c>
       <c r="N8" s="26" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="O8" s="26"/>
     </row>
@@ -2116,11 +3035,11 @@
         <v>0.25</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F10" s="22" t="s">
         <v>47</v>
@@ -2129,7 +3048,7 @@
         <v>40</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I10" s="22" t="s">
         <v>44</v>
@@ -2146,7 +3065,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="O10" s="22"/>
     </row>
@@ -2167,7 +3086,7 @@
         <v>41</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I11" s="22" t="s">
         <v>42</v>
@@ -2194,7 +3113,7 @@
         <v>0.25</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="21"/>
@@ -2205,7 +3124,7 @@
         <v>41</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I12" s="22" t="s">
         <v>44</v>
@@ -2222,7 +3141,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O12" s="22"/>
     </row>
@@ -2243,7 +3162,7 @@
         <v>41</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I13" s="22" t="s">
         <v>42</v>
@@ -2279,7 +3198,7 @@
         <v>41</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I14" s="22" t="s">
         <v>42</v>
@@ -2306,11 +3225,11 @@
         <v>0.2</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>47</v>
@@ -2319,7 +3238,7 @@
         <v>45</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I15" s="22" t="s">
         <v>44</v>
@@ -2336,32 +3255,32 @@
         <v>1</v>
       </c>
       <c r="N15" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O15" s="22"/>
     </row>
     <row r="16" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B16" s="20">
         <v>40000</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I16" s="22" t="s">
         <v>44</v>
@@ -2378,7 +3297,7 @@
         <v>1</v>
       </c>
       <c r="N16" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O16" s="22"/>
     </row>
@@ -2390,11 +3309,11 @@
         <v>0.80630000000000002</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D17" s="34"/>
       <c r="E17" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F17" s="22" t="s">
         <v>32</v>
@@ -2403,7 +3322,7 @@
         <v>46</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I17" s="22" t="s">
         <v>44</v>
@@ -2420,7 +3339,7 @@
         <v>1</v>
       </c>
       <c r="N17" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O17" s="22"/>
     </row>
@@ -2434,7 +3353,7 @@
       <c r="C18" s="33"/>
       <c r="D18" s="34"/>
       <c r="E18" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F18" s="22" t="s">
         <v>32</v>
@@ -2443,7 +3362,7 @@
         <v>41</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I18" s="22" t="s">
         <v>44</v>
@@ -2460,7 +3379,7 @@
         <v>1</v>
       </c>
       <c r="N18" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O18" s="22"/>
     </row>
@@ -2472,11 +3391,11 @@
         <v>0.40629999999999999</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19" s="34"/>
       <c r="E19" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F19" s="22" t="s">
         <v>32</v>
@@ -2485,7 +3404,7 @@
         <v>41</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I19" s="22" t="s">
         <v>44</v>
@@ -2502,7 +3421,7 @@
         <v>1</v>
       </c>
       <c r="N19" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O19" s="22"/>
     </row>
@@ -2516,7 +3435,7 @@
       <c r="C20" s="33"/>
       <c r="D20" s="34"/>
       <c r="E20" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F20" s="22" t="s">
         <v>32</v>
@@ -2525,7 +3444,7 @@
         <v>41</v>
       </c>
       <c r="H20" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I20" s="22" t="s">
         <v>42</v>
@@ -2553,17 +3472,17 @@
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E21" s="21"/>
       <c r="F21" s="22" t="s">
         <v>32</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H21" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I21" s="22" t="s">
         <v>42</v>
@@ -2590,11 +3509,11 @@
         <v>0.4</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F22" s="22" t="s">
         <v>32</v>
@@ -2603,7 +3522,7 @@
         <v>48</v>
       </c>
       <c r="H22" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I22" s="22" t="s">
         <v>44</v>
@@ -2620,22 +3539,22 @@
         <v>1</v>
       </c>
       <c r="N22" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O22" s="22"/>
     </row>
     <row r="23" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="B23" s="20">
         <v>0.19</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E23" s="21"/>
       <c r="F23" s="22" t="s">
@@ -2645,7 +3564,7 @@
         <v>49</v>
       </c>
       <c r="H23" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I23" s="22" t="s">
         <v>42</v>
@@ -2662,10 +3581,10 @@
         <v>0</v>
       </c>
       <c r="M23" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N23" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O23" s="22"/>
     </row>
@@ -2674,13 +3593,13 @@
         <v>54</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D24" s="37" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E24" s="21"/>
       <c r="F24" s="22" t="s">
@@ -2690,7 +3609,7 @@
         <v>56</v>
       </c>
       <c r="H24" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I24" s="22" t="s">
         <v>42</v>
@@ -2707,10 +3626,10 @@
         <v>0</v>
       </c>
       <c r="M24" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N24" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O24" s="22"/>
     </row>
@@ -2722,10 +3641,10 @@
         <v>58</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E25" s="21"/>
       <c r="F25" s="22" t="s">
@@ -2735,7 +3654,7 @@
         <v>57</v>
       </c>
       <c r="H25" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I25" s="22" t="s">
         <v>42</v>
@@ -2752,25 +3671,25 @@
         <v>0</v>
       </c>
       <c r="M25" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N25" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O25" s="22"/>
     </row>
     <row r="26" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E26" s="21"/>
       <c r="F26" s="22" t="s">
@@ -2780,7 +3699,7 @@
         <v>49</v>
       </c>
       <c r="H26" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I26" s="22" t="s">
         <v>44</v>
@@ -2797,10 +3716,10 @@
         <v>0</v>
       </c>
       <c r="M26" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N26" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O26" s="22"/>
     </row>
@@ -2809,16 +3728,16 @@
         <v>52</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D27" s="37" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F27" s="22" t="s">
         <v>32</v>
@@ -2827,7 +3746,7 @@
         <v>50</v>
       </c>
       <c r="H27" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I27" s="22" t="s">
         <v>42</v>
@@ -2844,7 +3763,7 @@
         <v>1</v>
       </c>
       <c r="N27" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O27" s="22"/>
     </row>
@@ -2856,13 +3775,13 @@
         <v>58</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D28" s="37" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F28" s="22" t="s">
         <v>32</v>
@@ -2871,7 +3790,7 @@
         <v>51</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I28" s="22" t="s">
         <v>42</v>
@@ -2888,32 +3807,32 @@
         <v>1</v>
       </c>
       <c r="N28" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O28" s="22"/>
     </row>
     <row r="29" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="22" t="s">
         <v>32</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I29" s="22" t="s">
         <v>44</v>
@@ -2930,32 +3849,32 @@
         <v>0</v>
       </c>
       <c r="M29" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N29" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O29" s="22"/>
     </row>
     <row r="30" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D30" s="37" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F30" s="22"/>
       <c r="H30" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I30" s="22" t="s">
         <v>42</v>
@@ -2972,29 +3891,29 @@
         <v>1</v>
       </c>
       <c r="N30" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O30" s="22"/>
     </row>
     <row r="31" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F31" s="22"/>
       <c r="H31" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I31" s="22" t="s">
         <v>42</v>
@@ -3011,7 +3930,7 @@
         <v>1</v>
       </c>
       <c r="N31" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O31" s="22"/>
     </row>
@@ -3031,16 +3950,16 @@
     </row>
     <row r="33" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C33" s="35" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D33" s="35" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E33" s="16"/>
       <c r="F33" s="17" t="s">
@@ -3050,7 +3969,7 @@
         <v>59</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I33" s="17" t="s">
         <v>42</v>
@@ -3067,33 +3986,33 @@
         <v>0</v>
       </c>
       <c r="M33" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N33" s="17"/>
       <c r="O33" s="17"/>
     </row>
     <row r="34" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B34" s="18">
         <v>1.5</v>
       </c>
       <c r="C34" s="35" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D34" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E34" s="16"/>
       <c r="F34" s="17" t="s">
         <v>60</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I34" s="17" t="s">
         <v>42</v>
@@ -3120,13 +4039,13 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D35" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F35" s="17" t="s">
         <v>62</v>
@@ -3135,7 +4054,7 @@
         <v>61</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I35" s="17" t="s">
         <v>42</v>
@@ -3162,20 +4081,22 @@
         <v>120</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D36" s="16"/>
+        <v>218</v>
+      </c>
+      <c r="D36" s="50" t="s">
+        <v>217</v>
+      </c>
       <c r="E36" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>64</v>
+        <v>215</v>
       </c>
       <c r="G36" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I36" s="17" t="s">
         <v>44</v>
@@ -3196,23 +4117,23 @@
     </row>
     <row r="37" spans="1:15" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B37" s="36">
         <v>1</v>
       </c>
       <c r="C37" s="35" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D37" s="35"/>
       <c r="E37" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F37" s="39" t="s">
         <v>33</v>
       </c>
       <c r="H37" s="39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I37" s="39" t="s">
         <v>44</v>
@@ -3231,359 +4152,251 @@
       <c r="N37" s="39"/>
       <c r="O37" s="39"/>
     </row>
-    <row r="38" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="41"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-      <c r="J38" s="43"/>
-      <c r="K38" s="43"/>
-      <c r="L38" s="43"/>
-      <c r="N38" s="43"/>
-      <c r="O38" s="43"/>
-    </row>
-    <row r="39" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="B39" s="41"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
-      <c r="K39" s="43"/>
-      <c r="L39" s="43"/>
-      <c r="N39" s="43"/>
-      <c r="O39" s="43"/>
-    </row>
-    <row r="40" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="41"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="43"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="43"/>
-      <c r="J40" s="43"/>
-      <c r="K40" s="43"/>
-      <c r="L40" s="43"/>
-      <c r="N40" s="43"/>
-      <c r="O40" s="43"/>
-    </row>
-    <row r="41" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H41" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="I41" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="J41" s="13">
-        <f t="shared" ref="J41:J42" si="5">IF(I41="Yes", 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="K41" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="L41" s="13">
-        <f t="shared" ref="L41:L42" si="6">IF(K41="Yes", 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="N41" s="13"/>
-      <c r="O41" s="13"/>
-    </row>
-    <row r="42" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="H42" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="I42" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="J42" s="13">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="K42" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="L42" s="13">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="N42" s="13"/>
-      <c r="O42" s="13"/>
-    </row>
-    <row r="43" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B43" s="11">
-        <v>32</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="H43" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="I43" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="J43" s="13">
-        <f t="shared" ref="J43:J48" si="7">IF(I43="Yes", 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="K43" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="L43" s="13">
-        <f t="shared" ref="L43:L48" si="8">IF(K43="Yes", 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="N43" s="13"/>
-      <c r="O43" s="13"/>
-    </row>
-    <row r="44" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B44" s="11">
-        <v>-2.9</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="H44" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="I44" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="J44" s="13">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="K44" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="L44" s="13">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="N44" s="13"/>
-      <c r="O44" s="13"/>
+    <row r="38" spans="1:15" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="36"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="39"/>
+      <c r="L38" s="39"/>
+      <c r="N38" s="39"/>
+      <c r="O38" s="39"/>
+    </row>
+    <row r="39" spans="1:15" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="B39" s="36"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="39"/>
+      <c r="N39" s="39"/>
+      <c r="O39" s="39"/>
+    </row>
+    <row r="40" spans="1:15" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="36"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="39"/>
+      <c r="H40" s="39"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="39"/>
+      <c r="L40" s="39"/>
+      <c r="N40" s="39"/>
+      <c r="O40" s="39"/>
+    </row>
+    <row r="41" spans="1:15" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="36"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="39"/>
+      <c r="L41" s="39"/>
+      <c r="N41" s="39"/>
+      <c r="O41" s="39"/>
+    </row>
+    <row r="42" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="41"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="43"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="43"/>
+      <c r="N42" s="43"/>
+      <c r="O42" s="43"/>
+    </row>
+    <row r="43" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="B43" s="41"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="43"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
+      <c r="K43" s="43"/>
+      <c r="L43" s="43"/>
+      <c r="N43" s="43"/>
+      <c r="O43" s="43"/>
+    </row>
+    <row r="44" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="41"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="43"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
+      <c r="K44" s="43"/>
+      <c r="L44" s="43"/>
+      <c r="N44" s="43"/>
+      <c r="O44" s="43"/>
     </row>
     <row r="45" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="11">
-        <v>0.5</v>
+        <v>125</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
       <c r="F45" s="13" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I45" s="13" t="s">
         <v>44</v>
       </c>
       <c r="J45" s="13">
+        <f t="shared" ref="J45:J46" si="5">IF(I45="Yes", 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="K45" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L45" s="13">
+        <f t="shared" ref="L45:L46" si="6">IF(K45="Yes", 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="N45" s="13"/>
+      <c r="O45" s="13"/>
+    </row>
+    <row r="46" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="J46" s="13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K46" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L46" s="13">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
+    </row>
+    <row r="47" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="11">
+        <v>32</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="J47" s="13">
+        <f t="shared" ref="J47:J52" si="7">IF(I47="Yes", 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="K47" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L47" s="13">
+        <f t="shared" ref="L47:L52" si="8">IF(K47="Yes", 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="N47" s="13"/>
+      <c r="O47" s="13"/>
+    </row>
+    <row r="48" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="11">
+        <v>-2.9</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="J48" s="13">
         <f t="shared" si="7"/>
         <v>1</v>
-      </c>
-      <c r="K45" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="L45" s="13">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="N45" s="13"/>
-      <c r="O45" s="13"/>
-    </row>
-    <row r="46" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B46" s="11">
-        <v>0.42</v>
-      </c>
-      <c r="C46" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="D46" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="F46" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="H46" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="I46" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J46" s="13">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K46" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="L46" s="13">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="M46" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="N46" s="13"/>
-      <c r="O46" s="13"/>
-    </row>
-    <row r="47" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B47" s="11">
-        <v>0.4</v>
-      </c>
-      <c r="C47" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="D47" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="F47" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G47" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H47" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="I47" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J47" s="13">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K47" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="L47" s="13">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="N47" s="13"/>
-      <c r="O47" s="13"/>
-    </row>
-    <row r="48" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="B48" s="11">
-        <v>0.38</v>
-      </c>
-      <c r="C48" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="D48" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="F48" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H48" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="I48" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J48" s="13">
-        <f t="shared" si="7"/>
-        <v>0</v>
       </c>
       <c r="K48" s="13" t="s">
         <v>44</v>
@@ -3595,182 +4408,205 @@
       <c r="N48" s="13"/>
       <c r="O48" s="13"/>
     </row>
-    <row r="49" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="41"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="43"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
-      <c r="J49" s="43"/>
-      <c r="K49" s="43"/>
-      <c r="L49" s="43"/>
-      <c r="N49" s="43"/>
-      <c r="O49" s="43"/>
-    </row>
-    <row r="50" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" s="28">
-        <v>283.79599999999999</v>
-      </c>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="G50" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="H50" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="I50" s="30" t="s">
+    <row r="49" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I49" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="J49" s="13">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="K49" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L49" s="13">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N49" s="13"/>
+      <c r="O49" s="13"/>
+    </row>
+    <row r="50" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" s="11">
+        <v>0.42</v>
+      </c>
+      <c r="C50" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F50" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="I50" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="J50" s="30">
-        <f t="shared" si="0"/>
+      <c r="J50" s="13">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K50" s="30" t="s">
+      <c r="K50" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L50" s="13">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M50" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="N50" s="13"/>
+      <c r="O50" s="13"/>
+    </row>
+    <row r="51" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B51" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="C51" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="D51" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H51" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="I51" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="L50" s="30">
-        <f t="shared" si="1"/>
+      <c r="J51" s="13">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="N50" s="30"/>
-      <c r="O50" s="30"/>
-    </row>
-    <row r="51" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="27" t="s">
+      <c r="K51" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L51" s="13">
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="B51" s="28">
-        <v>1.1237199999999999E-2</v>
-      </c>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="G51" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="H51" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="I51" s="30" t="s">
+      <c r="N51" s="13"/>
+      <c r="O51" s="13"/>
+    </row>
+    <row r="52" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B52" s="11">
+        <v>0.38</v>
+      </c>
+      <c r="C52" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="D52" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H52" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="I52" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="J51" s="30">
-        <f>IF(I51="Yes", 1, 0)</f>
+      <c r="J52" s="13">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K51" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="L51" s="30">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N51" s="30"/>
-      <c r="O51" s="30"/>
-    </row>
-    <row r="52" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" s="28">
-        <v>20</v>
-      </c>
-      <c r="C52" s="29"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="G52" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="H52" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="I52" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="J52" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K52" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="L52" s="30">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N52" s="30"/>
-      <c r="O52" s="30"/>
-    </row>
-    <row r="53" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="B53" s="28">
-        <v>23.91</v>
-      </c>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="G53" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="H53" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="I53" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="J53" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K53" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="L53" s="30">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N53" s="30"/>
-      <c r="O53" s="30"/>
+      <c r="K52" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L52" s="13">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N52" s="13"/>
+      <c r="O52" s="13"/>
+    </row>
+    <row r="53" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="41"/>
+      <c r="C53" s="42"/>
+      <c r="D53" s="42"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="43"/>
+      <c r="H53" s="43"/>
+      <c r="I53" s="43"/>
+      <c r="J53" s="43"/>
+      <c r="K53" s="43"/>
+      <c r="L53" s="43"/>
+      <c r="N53" s="43"/>
+      <c r="O53" s="43"/>
     </row>
     <row r="54" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="27" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B54" s="28">
-        <v>8.3140000000000002E-3</v>
+        <v>283.79599999999999</v>
       </c>
       <c r="C54" s="29"/>
       <c r="D54" s="29"/>
       <c r="E54" s="29"/>
       <c r="F54" s="30" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G54" s="27" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="H54" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I54" s="30" t="s">
         <v>42</v>
@@ -3791,22 +4627,22 @@
     </row>
     <row r="55" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="27" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B55" s="28">
-        <v>42600</v>
+        <v>1.1237199999999999E-2</v>
       </c>
       <c r="C55" s="29"/>
       <c r="D55" s="29"/>
       <c r="E55" s="29"/>
       <c r="F55" s="30" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G55" s="27" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="H55" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I55" s="30" t="s">
         <v>42</v>
@@ -3819,131 +4655,287 @@
         <v>42</v>
       </c>
       <c r="L55" s="30">
-        <f>IF(K55="Yes", 1, 0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N55" s="30"/>
       <c r="O55" s="30"/>
     </row>
-    <row r="56" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="41"/>
-      <c r="C56" s="42"/>
-      <c r="D56" s="42"/>
-      <c r="E56" s="42"/>
-      <c r="F56" s="43"/>
-      <c r="H56" s="43"/>
-      <c r="I56" s="43"/>
-      <c r="J56" s="43"/>
-      <c r="K56" s="43"/>
-      <c r="L56" s="43"/>
-      <c r="N56" s="43"/>
-      <c r="O56" s="43"/>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J57" s="2">
-        <f>SUM(J2:J55)</f>
+    <row r="56" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="28">
+        <v>20</v>
+      </c>
+      <c r="C56" s="29"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="G56" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="H56" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="I56" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="J56" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K56" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="L56" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N56" s="30"/>
+      <c r="O56" s="30"/>
+    </row>
+    <row r="57" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" s="28">
+        <v>23.91</v>
+      </c>
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="G57" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H57" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="I57" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="J57" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K57" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="L57" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N57" s="30"/>
+      <c r="O57" s="30"/>
+    </row>
+    <row r="58" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="28">
+        <v>8.3140000000000002E-3</v>
+      </c>
+      <c r="C58" s="29"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="29"/>
+      <c r="F58" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="G58" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="H58" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="I58" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="J58" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K58" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="L58" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N58" s="30"/>
+      <c r="O58" s="30"/>
+    </row>
+    <row r="59" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" s="28">
+        <v>42600</v>
+      </c>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G59" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="H59" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="I59" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="J59" s="30">
+        <f>IF(I59="Yes", 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K59" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="L59" s="30">
+        <f>IF(K59="Yes", 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N59" s="30"/>
+      <c r="O59" s="30"/>
+    </row>
+    <row r="60" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="41"/>
+      <c r="C60" s="42"/>
+      <c r="D60" s="42"/>
+      <c r="E60" s="42"/>
+      <c r="F60" s="43"/>
+      <c r="H60" s="43"/>
+      <c r="I60" s="43"/>
+      <c r="J60" s="43"/>
+      <c r="K60" s="43"/>
+      <c r="L60" s="43"/>
+      <c r="N60" s="43"/>
+      <c r="O60" s="43"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J61" s="2">
+        <f>SUM(J2:J59)</f>
         <v>18</v>
       </c>
-      <c r="K57" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="L57" s="2">
-        <f>SUM(L2:L55)</f>
+      <c r="K61" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="L61" s="2">
+        <f>SUM(L2:L59)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="5">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="5">
         <v>1</v>
       </c>
-      <c r="B59" s="4">
-        <f>EXP(-A59*10)</f>
+      <c r="B63" s="4">
+        <f>EXP(-A63*10)</f>
         <v>4.5399929762484854E-5</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="C63" s="49">
+        <f>50*0.01</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>0.1</v>
       </c>
-      <c r="B60" s="4">
-        <f t="shared" ref="B60:B61" si="9">EXP(-A60*10)</f>
+      <c r="B64" s="4">
+        <f t="shared" ref="B64:B65" si="9">EXP(-A64*10)</f>
         <v>0.36787944117144233</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
+      <c r="C64" s="4"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="5">
         <v>0.01</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B65" s="4">
         <f t="shared" si="9"/>
         <v>0.90483741803595952</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="6"/>
-      <c r="H63" s="6"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="6"/>
-      <c r="K63" s="2"/>
-      <c r="N63" s="6"/>
-      <c r="O63" s="6"/>
+      <c r="C65" s="4"/>
+    </row>
+    <row r="67" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="2"/>
+      <c r="N67" s="6"/>
+      <c r="O67" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K59:K63 I2:I10 K51:K55 I57:I63 K33:K37 I33:I37 K41:K42 I50:I55 I15:I25 I41:I48 K2:K25 K45:K48 K27:K28 I27:I28 I30:I31 K30:K31">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+  <conditionalFormatting sqref="K63:K67 I2:I10 K55:K59 I61:I67 K33:K41 I33:I41 K45:K46 I54:I59 I15:I25 I45:I52 K2:K25 K49:K52 K27:K28 I27:I28 I30:I31 K30:K31">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K50">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+  <conditionalFormatting sqref="K54">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K43:K44">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+  <conditionalFormatting sqref="K47:K48">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:I14">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I56 K56 I49 K49 I38:I40 K38:K40 I32 K32">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="I60 K60 I53 K53 I42:I44 K42:K44 I32 K32">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26 K26">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29 K29">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D36" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J40"/>
+  <dimension ref="A2:J45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3956,25 +4948,25 @@
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F2" t="s">
         <v>170</v>
       </c>
-      <c r="E2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F2" t="s">
-        <v>172</v>
-      </c>
       <c r="J2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -4000,7 +4992,7 @@
         <v>41.666666666666664</v>
       </c>
       <c r="I3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J3">
         <f>100*0.5/24</f>
@@ -4021,235 +5013,549 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>169</v>
-      </c>
-      <c r="C6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>211</v>
+      </c>
+      <c r="E7" s="6">
+        <v>14</v>
+      </c>
+      <c r="F7" s="6">
+        <v>16</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>212</v>
+      </c>
+      <c r="E8" s="6">
+        <v>16</v>
+      </c>
+      <c r="F8" s="6">
+        <v>17</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>160</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C9" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="C7">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>159</v>
-      </c>
-      <c r="B8" t="s">
-        <v>166</v>
-      </c>
-      <c r="C8">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>158</v>
-      </c>
-      <c r="B9" t="s">
-        <v>166</v>
-      </c>
-      <c r="C9">
-        <v>21</v>
-      </c>
+      <c r="D9" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E9" s="6">
+        <f>E8-E7</f>
+        <v>2</v>
+      </c>
+      <c r="F9" s="6">
+        <f>F8-F7</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10">
+        <v>21</v>
+      </c>
+      <c r="E10" s="2">
+        <f>50*$E$9</f>
+        <v>100</v>
+      </c>
+      <c r="F10" s="2">
+        <f>50*$E$9</f>
+        <v>100</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>157</v>
       </c>
-      <c r="B10" t="s">
-        <v>166</v>
-      </c>
-      <c r="C10">
-        <v>10</v>
-      </c>
+      <c r="B11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11">
+        <v>21</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" ref="E11:F14" si="0">50*$E$9</f>
+        <v>100</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>156</v>
       </c>
       <c r="B12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C12">
-        <v>10</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B13" t="s">
         <v>164</v>
       </c>
       <c r="C13">
-        <v>8</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>163</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="B14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2">
+        <f>50*$E$9</f>
+        <v>100</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C15">
-        <v>5</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B16" t="s">
         <v>162</v>
       </c>
       <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>161</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>146</v>
+        <v>148</v>
+      </c>
+      <c r="B19" t="s">
+        <v>160</v>
       </c>
       <c r="C19">
-        <f>SUM(C7:D17)</f>
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>160</v>
-      </c>
-      <c r="B23" t="s">
-        <v>153</v>
-      </c>
-      <c r="C23">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22">
+        <f>SUM(C10:D20)</f>
+        <v>104</v>
+      </c>
+      <c r="E22" s="2">
+        <f>SUM(E10:E20)</f>
+        <v>500</v>
+      </c>
+      <c r="F22" s="2">
+        <f>SUM(F10:F20)</f>
+        <v>500</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2">
+        <f>F22+E22</f>
+        <v>1000</v>
+      </c>
+      <c r="G23" s="2">
+        <f>G22+F22</f>
+        <v>500</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B24" t="s">
-        <v>153</v>
-      </c>
-      <c r="C24">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>158</v>
       </c>
-      <c r="B25" t="s">
-        <v>153</v>
-      </c>
-      <c r="C25">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>157</v>
-      </c>
       <c r="B26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C26">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>157</v>
+      </c>
+      <c r="B27" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>156</v>
       </c>
-      <c r="B27" t="s">
-        <v>155</v>
-      </c>
-      <c r="C27">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>154</v>
-      </c>
       <c r="B28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C28">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="46" t="s">
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>154</v>
+      </c>
+      <c r="B30" t="s">
+        <v>153</v>
+      </c>
+      <c r="C30">
+        <v>7</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>152</v>
       </c>
-      <c r="B29" s="46" t="s">
+      <c r="B31" t="s">
         <v>151</v>
       </c>
-      <c r="C29" s="46">
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="C32" s="46">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>150</v>
-      </c>
-      <c r="B30" t="s">
-        <v>149</v>
-      </c>
-      <c r="C30">
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33" t="s">
+        <v>147</v>
+      </c>
+      <c r="C33">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>148</v>
-      </c>
-      <c r="B31" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>146</v>
       </c>
-      <c r="C32">
-        <f>SUM(C23:D30)</f>
+      <c r="B34" t="s">
+        <v>145</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>144</v>
+      </c>
+      <c r="C35">
+        <f>SUM(C26:D33)</f>
         <v>96</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>146</v>
-      </c>
-      <c r="C40">
-        <f>SUM(C19,C32)</f>
-        <v>197</v>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38">
+        <f>SUM(C22,C35)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C42" s="2">
+        <v>24</v>
+      </c>
+      <c r="D42" s="2">
+        <f>A45/24</f>
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f>1.5*B45</f>
+        <v>294</v>
+      </c>
+      <c r="B45">
+        <f>C45*D45</f>
+        <v>196</v>
+      </c>
+      <c r="C45">
+        <f>14*2</f>
+        <v>28</v>
+      </c>
+      <c r="D45">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ready for Morris graphs
</commit_message>
<xml_diff>
--- a/WriteUp/ParamTests/ParameterTests.xlsx
+++ b/WriteUp/ParamTests/ParameterTests.xlsx
@@ -2138,8 +2138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
LHS ready for testing
</commit_message>
<xml_diff>
--- a/WriteUp/ParamTests/ParameterTests.xlsx
+++ b/WriteUp/ParamTests/ParameterTests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="7965" yWindow="480" windowWidth="19935" windowHeight="12240"/>
+    <workbookView xWindow="7965" yWindow="480" windowWidth="16035" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="3" r:id="rId1"/>
@@ -55,6 +55,32 @@
 Two TSS to be produced:
 a) Cumulative only during obs. concentration
 b) Cumulative for the model duration</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>pablo alvarez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Decided not do produce these TSS, as the comparison to the filed estimations is of no sense given that the application regime considered in the model is significantly different than that assumed by the field sampling.
+However, what should be of insterest is comparison of the degraded estimations (based on the field Epsilon).
+To compare the leaching component the transect pixels will be used for comparison. </t>
         </r>
       </text>
     </comment>
@@ -117,7 +143,8 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">EU Commision
+          <t xml:space="preserve">Lefranqc: 7 - 16180
+EU Commision
 Koc (S-metolachlor) : 110-369, median : 226 l/kg
 IUPAC: 
 Literature value: Kd range 0.33-1.64 mL/g, Koc range 50.0-540 mL/g, soils=33; Other sources: 120.2-309.0 mL/g (R3), Log Koc 2.26 at 25 Deg C (R4)
@@ -170,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="298">
   <si>
     <t xml:space="preserve">epsilon_iso </t>
   </si>
@@ -568,27 +595,15 @@
     <t>$\theta_{SATz3+}$</t>
   </si>
   <si>
-    <t>0.53 (0.47 - 0.53)</t>
-  </si>
-  <si>
-    <t>0.01 - 0.05</t>
-  </si>
-  <si>
     <t>Conceptual</t>
   </si>
   <si>
-    <t>0.63 (0.54 - 0.61)</t>
-  </si>
-  <si>
     <t>Sens.</t>
   </si>
   <si>
     <t>Test</t>
   </si>
   <si>
-    <t>0.39 (0.34 - 0.41)</t>
-  </si>
-  <si>
     <t>Ouput TSS</t>
   </si>
   <si>
@@ -769,9 +784,6 @@
     <t>$\theta_{WPz2}$</t>
   </si>
   <si>
-    <t>0.16 (0.13 - 0.19)</t>
-  </si>
-  <si>
     <t>$\theta_{WPz3+}$</t>
   </si>
   <si>
@@ -824,9 +836,6 @@
   </si>
   <si>
     <t>https://sitem.herts.ac.uk/aeru/iupac/Reports/465.htm</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 50 - 540</t>
   </si>
   <si>
     <r>
@@ -982,36 +991,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Leached from Top Soil </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(z0 only)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Leached from 30 cm </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(z1)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Mass in</t>
     </r>
     <r>
@@ -1066,25 +1045,7 @@
     <t>Total catchment mass - Z (heavy &amp; light)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Runoff from Top soil </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(z0)</t>
-    </r>
-  </si>
-  <si>
     <t>Calculate from outlet components</t>
-  </si>
-  <si>
-    <t>Comments (if any)</t>
   </si>
   <si>
     <t>Aged</t>
@@ -2674,42 +2635,95 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Drainage (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>layer z1+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>Latflow mass flux. (heavy &amp; light)</t>
   </si>
   <si>
     <t>Area Transects Masses (heavy &amp; light)</t>
+  </si>
+  <si>
+    <t>Removed from Model</t>
+  </si>
+  <si>
+    <t>Morris -&gt; Fix</t>
+  </si>
+  <si>
+    <t>Fix -&gt;  0.19</t>
+  </si>
+  <si>
+    <t>Fix -&gt; 0.37</t>
+  </si>
+  <si>
+    <t>0.02 - 0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7 - 16180</t>
+  </si>
+  <si>
+    <t>resM_EXP_light_g_tss</t>
+  </si>
+  <si>
+    <t>resM_EXP_heavy_g_tss</t>
+  </si>
+  <si>
+    <t>resM_oCONC_ugL_tss</t>
+  </si>
+  <si>
+    <t>resM_oCONC_ROFF_ugL_tss</t>
+  </si>
+  <si>
+    <t>resM_oCONC_LF_ugL_tss</t>
+  </si>
+  <si>
+    <t>resM_oCONC_ADR_ugL_tss</t>
+  </si>
+  <si>
+    <t>No mass transport with Linear Reservoir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conc &amp; delta as output, </t>
+  </si>
+  <si>
+    <t>I can come back to masses if needed based on bulk densities and sampled pixels</t>
+  </si>
+  <si>
+    <t>resW_o_cellLatflow_m3.tss</t>
+  </si>
+  <si>
+    <t>resW_o_accDrain_m3.tss</t>
+  </si>
+  <si>
+    <t>Drainage (layer z2)</t>
+  </si>
+  <si>
+    <t>resW_accRunoff_m3.tss</t>
+  </si>
+  <si>
+    <t>resW_accBaseflow_m3.tss</t>
+  </si>
+  <si>
+    <t>resM_accAGED_DEGzX.tss</t>
+  </si>
+  <si>
+    <t>resM_accDEGzX.tss</t>
+  </si>
+  <si>
+    <t>Volat</t>
+  </si>
+  <si>
+    <t>z0 - only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leached from Top Soil </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runoff from Top soil </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2826,8 +2840,39 @@
       <family val="3"/>
     </font>
     <font>
+      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3091,7 +3136,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3275,7 +3320,49 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3717,10 +3804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3731,433 +3818,481 @@
     <col min="4" max="4" width="43.42578125" customWidth="1"/>
     <col min="5" max="5" width="45.5703125" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" style="85" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+      <c r="G1" s="84"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="75" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B5" s="75" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C5" s="75" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="75" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E5" s="76"/>
       <c r="F5" s="75"/>
-      <c r="G5" s="76" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="85"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="72" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B6" s="60" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C6" s="60" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D6" s="61" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="E6" s="61">
         <v>2</v>
       </c>
       <c r="F6" s="62"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="72"/>
       <c r="B7" s="61" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C7" s="60" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="D7" s="61" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="E7" s="61">
         <v>2</v>
       </c>
       <c r="F7" s="62"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="72"/>
       <c r="B8" s="61" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="C8" s="60" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="D8" s="61" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="E8" s="61">
         <v>2</v>
       </c>
       <c r="F8" s="62"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="68" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B9" s="60" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C9" s="60" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D9" s="61" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E9" s="61" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="F9" s="62"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="68" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B10" s="60" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D10" s="61" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="E10" s="61" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F10" s="62"/>
     </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="75" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B12" s="75"/>
       <c r="C12" s="75"/>
       <c r="D12" s="75"/>
       <c r="E12" s="76"/>
       <c r="F12" s="75"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="84"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="68" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B13" s="61" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C13" s="61" t="s">
+        <v>178</v>
+      </c>
+      <c r="D13" s="61" t="s">
+        <v>179</v>
+      </c>
+      <c r="E13" s="61" t="s">
+        <v>226</v>
+      </c>
+      <c r="F13" s="63" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="68" t="s">
         <v>182</v>
       </c>
-      <c r="D13" s="61" t="s">
-        <v>183</v>
-      </c>
-      <c r="E13" s="61" t="s">
-        <v>232</v>
-      </c>
-      <c r="F13" s="63" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="68" t="s">
-        <v>186</v>
-      </c>
       <c r="B14" s="61" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C14" s="61" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D14" s="61" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E14" s="61">
         <v>2</v>
       </c>
       <c r="F14" s="63"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="86" t="s">
+        <v>278</v>
+      </c>
+      <c r="H14" s="83" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="67" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D15" s="52" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E15" s="52" t="s">
         <v>32</v>
       </c>
       <c r="F15" s="66"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="86" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="69" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C16" s="52" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D16" s="52" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E16" s="52">
         <v>6</v>
       </c>
       <c r="F16" s="66" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="71"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="81" t="s">
-        <v>282</v>
-      </c>
-      <c r="E17" s="58">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="98" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="94"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="99" t="s">
+        <v>271</v>
+      </c>
+      <c r="E17" s="95">
         <v>6</v>
       </c>
-      <c r="F17" s="64"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="96"/>
+      <c r="G17" s="97"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="70"/>
       <c r="B18" s="55"/>
       <c r="C18" s="55"/>
       <c r="D18" s="55" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="F18" s="65"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="71" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C19" s="58" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D19" s="58" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E19" s="58" t="s">
         <v>32</v>
       </c>
       <c r="F19" s="64" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="G19" s="85" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="70"/>
       <c r="B20" s="55"/>
       <c r="C20" s="55"/>
       <c r="D20" s="55" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E20" s="55" t="s">
         <v>32</v>
       </c>
       <c r="F20" s="56"/>
-    </row>
-    <row r="22" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="85" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="75" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B22" s="75"/>
       <c r="C22" s="75"/>
       <c r="D22" s="75"/>
       <c r="E22" s="76"/>
       <c r="F22" s="75"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="84"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="67" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B23" s="52" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E23" s="52">
         <v>1</v>
       </c>
       <c r="F23" s="53"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="85" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="73"/>
       <c r="B24" s="58"/>
       <c r="C24" s="57"/>
-      <c r="D24" s="58" t="s">
-        <v>280</v>
+      <c r="D24" s="93" t="s">
+        <v>289</v>
       </c>
       <c r="E24" s="58">
         <v>1</v>
       </c>
       <c r="F24" s="59"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="85" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="73"/>
       <c r="B25" s="58"/>
       <c r="C25" s="57"/>
       <c r="D25" s="58" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E25" s="58">
         <v>1</v>
       </c>
       <c r="F25" s="59"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="85" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="74"/>
       <c r="B26" s="55"/>
       <c r="C26" s="54"/>
       <c r="D26" s="55" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="E26" s="55">
         <v>1</v>
       </c>
       <c r="F26" s="56"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="85" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="67" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B27" s="52" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D27" s="52" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="E27" s="52">
         <v>2</v>
       </c>
       <c r="F27" s="53"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="86" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="73"/>
       <c r="B28" s="58"/>
       <c r="C28" s="57"/>
       <c r="D28" s="58" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="E28" s="58">
         <v>2</v>
       </c>
       <c r="F28" s="59"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="85" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="73"/>
       <c r="B29" s="58"/>
       <c r="C29" s="57"/>
       <c r="D29" s="58" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="E29" s="58">
         <v>2</v>
       </c>
       <c r="F29" s="59"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="74"/>
-      <c r="B30" s="55"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="55" t="s">
-        <v>242</v>
-      </c>
-      <c r="E30" s="55">
-        <v>2</v>
-      </c>
-      <c r="F30" s="56"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="85" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="87"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="99" t="s">
+        <v>236</v>
+      </c>
+      <c r="E30" s="99" t="s">
+        <v>284</v>
+      </c>
+      <c r="F30" s="90"/>
+      <c r="G30" s="91"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="69" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B31" s="52" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D31" s="52" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="E31" s="52">
         <v>6</v>
       </c>
       <c r="F31" s="53"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="70"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="70" t="s">
+        <v>295</v>
+      </c>
       <c r="B32" s="55"/>
       <c r="C32" s="54"/>
       <c r="D32" s="55" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E32" s="55">
         <v>2</v>
       </c>
       <c r="F32" s="56"/>
+      <c r="G32" s="85" t="s">
+        <v>293</v>
+      </c>
+      <c r="H32" s="85" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="69"/>
       <c r="B33" s="52"/>
       <c r="C33" s="51" t="s">
-        <v>249</v>
+        <v>296</v>
       </c>
       <c r="D33" s="52" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="E33" s="52">
         <v>2</v>
@@ -4168,7 +4303,9 @@
       <c r="A34" s="70"/>
       <c r="B34" s="55"/>
       <c r="C34" s="54"/>
-      <c r="D34" s="55"/>
+      <c r="D34" s="55" t="s">
+        <v>242</v>
+      </c>
       <c r="E34" s="55"/>
       <c r="F34" s="56"/>
     </row>
@@ -4176,13 +4313,13 @@
       <c r="A35" s="69"/>
       <c r="B35" s="52"/>
       <c r="C35" s="51" t="s">
-        <v>250</v>
+        <v>297</v>
       </c>
       <c r="D35" s="52" t="s">
-        <v>248</v>
-      </c>
-      <c r="E35" s="52">
-        <v>2</v>
+        <v>241</v>
+      </c>
+      <c r="E35" s="52" t="s">
+        <v>246</v>
       </c>
       <c r="F35" s="53"/>
     </row>
@@ -4190,40 +4327,42 @@
       <c r="A36" s="70"/>
       <c r="B36" s="55"/>
       <c r="C36" s="54"/>
-      <c r="D36" s="55"/>
+      <c r="D36" s="55" t="s">
+        <v>242</v>
+      </c>
       <c r="E36" s="55"/>
       <c r="F36" s="56"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="69"/>
-      <c r="B37" s="52"/>
-      <c r="C37" s="51" t="s">
-        <v>254</v>
+      <c r="A37" s="71"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="57" t="s">
+        <v>294</v>
       </c>
       <c r="D37" s="52" t="s">
-        <v>248</v>
-      </c>
-      <c r="E37" s="52" t="s">
-        <v>255</v>
-      </c>
-      <c r="F37" s="53"/>
+        <v>241</v>
+      </c>
+      <c r="E37" s="58"/>
+      <c r="F37" s="59"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="70"/>
-      <c r="B38" s="55"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="56"/>
+      <c r="A38" s="71"/>
+      <c r="B38" s="58"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="55" t="s">
+        <v>242</v>
+      </c>
+      <c r="E38" s="58"/>
+      <c r="F38" s="59"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="69"/>
       <c r="B39" s="52"/>
       <c r="C39" s="51" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="D39" s="52" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="E39" s="52"/>
       <c r="F39" s="53"/>
@@ -4232,7 +4371,9 @@
       <c r="A40" s="70"/>
       <c r="B40" s="55"/>
       <c r="C40" s="54"/>
-      <c r="D40" s="55"/>
+      <c r="D40" s="55" t="s">
+        <v>242</v>
+      </c>
       <c r="E40" s="55"/>
       <c r="F40" s="56"/>
     </row>
@@ -4273,10 +4414,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O67"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50:D52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4307,7 +4448,7 @@
         <v>123</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>30</v>
@@ -4330,10 +4471,10 @@
         <v>108</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -4345,7 +4486,7 @@
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E2" s="25"/>
       <c r="F2" s="26" t="s">
@@ -4383,7 +4524,7 @@
       </c>
       <c r="C3" s="25"/>
       <c r="D3" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="26" t="s">
@@ -4421,7 +4562,7 @@
       </c>
       <c r="C4" s="25"/>
       <c r="D4" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E4" s="25"/>
       <c r="F4" s="26" t="s">
@@ -4459,7 +4600,7 @@
       </c>
       <c r="C5" s="25"/>
       <c r="D5" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E5" s="25"/>
       <c r="F5" s="26" t="s">
@@ -4497,7 +4638,7 @@
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E6" s="25"/>
       <c r="F6" s="26" t="s">
@@ -4535,7 +4676,7 @@
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="26" t="s">
@@ -4602,7 +4743,7 @@
         <v>1</v>
       </c>
       <c r="N8" s="26" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="O8" s="26"/>
     </row>
@@ -4658,7 +4799,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="22" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="O10" s="22"/>
     </row>
@@ -4734,7 +4875,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O12" s="22"/>
     </row>
@@ -4848,7 +4989,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O15" s="22"/>
     </row>
@@ -4890,7 +5031,7 @@
         <v>1</v>
       </c>
       <c r="N16" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O16" s="22"/>
     </row>
@@ -4932,7 +5073,7 @@
         <v>1</v>
       </c>
       <c r="N17" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O17" s="22"/>
     </row>
@@ -4958,11 +5099,11 @@
         <v>92</v>
       </c>
       <c r="I18" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J18" s="22">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" s="47" t="s">
         <v>44</v>
@@ -4972,7 +5113,7 @@
         <v>1</v>
       </c>
       <c r="N18" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O18" s="22"/>
     </row>
@@ -5014,7 +5155,7 @@
         <v>1</v>
       </c>
       <c r="N19" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O19" s="22"/>
     </row>
@@ -5065,7 +5206,7 @@
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E21" s="21"/>
       <c r="F21" s="22" t="s">
@@ -5132,13 +5273,13 @@
         <v>1</v>
       </c>
       <c r="N22" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O22" s="22"/>
     </row>
     <row r="23" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B23" s="20">
         <v>0.19</v>
@@ -5177,7 +5318,7 @@
         <v>84</v>
       </c>
       <c r="N23" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O23" s="22"/>
     </row>
@@ -5222,7 +5363,7 @@
         <v>84</v>
       </c>
       <c r="N24" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O24" s="22"/>
     </row>
@@ -5267,24 +5408,26 @@
         <v>84</v>
       </c>
       <c r="N25" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O25" s="22"/>
     </row>
     <row r="26" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>199</v>
+        <v>193</v>
+      </c>
+      <c r="C26" s="82" t="s">
+        <v>274</v>
       </c>
       <c r="D26" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="E26" s="21"/>
+      <c r="E26" s="21" t="s">
+        <v>273</v>
+      </c>
       <c r="F26" s="22" t="s">
         <v>32</v>
       </c>
@@ -5295,24 +5438,24 @@
         <v>92</v>
       </c>
       <c r="I26" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J26" s="22">
         <f t="shared" ref="J26" si="2">IF(I26="Yes", 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" s="47" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L26" s="22">
         <f t="shared" ref="L26" si="3">IF(K26="Yes", 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26" s="19" t="s">
         <v>84</v>
       </c>
       <c r="N26" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O26" s="22"/>
     </row>
@@ -5323,14 +5466,14 @@
       <c r="B27" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="C27" s="37" t="s">
-        <v>138</v>
+      <c r="C27" s="82" t="s">
+        <v>275</v>
       </c>
       <c r="D27" s="37" t="s">
         <v>124</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F27" s="22" t="s">
         <v>32</v>
@@ -5356,7 +5499,7 @@
         <v>1</v>
       </c>
       <c r="N27" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O27" s="22"/>
     </row>
@@ -5367,14 +5510,14 @@
       <c r="B28" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="37" t="s">
-        <v>135</v>
+      <c r="C28" s="82" t="s">
+        <v>274</v>
       </c>
       <c r="D28" s="37" t="s">
         <v>124</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F28" s="22" t="s">
         <v>32</v>
@@ -5400,19 +5543,19 @@
         <v>1</v>
       </c>
       <c r="N28" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O28" s="22"/>
     </row>
     <row r="29" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>199</v>
+        <v>193</v>
+      </c>
+      <c r="C29" s="82" t="s">
+        <v>274</v>
       </c>
       <c r="D29" s="21" t="s">
         <v>121</v>
@@ -5422,30 +5565,30 @@
         <v>32</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H29" s="22" t="s">
         <v>92</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J29" s="22">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29" s="47" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L29" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M29" s="19" t="s">
         <v>84</v>
       </c>
       <c r="N29" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O29" s="22"/>
     </row>
@@ -5456,14 +5599,14 @@
       <c r="B30" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="C30" s="37" t="s">
-        <v>138</v>
+      <c r="C30" s="82" t="s">
+        <v>275</v>
       </c>
       <c r="D30" s="37" t="s">
         <v>124</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F30" s="22"/>
       <c r="H30" s="22" t="s">
@@ -5484,7 +5627,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O30" s="22"/>
     </row>
@@ -5495,14 +5638,14 @@
       <c r="B31" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="C31" s="37" t="s">
-        <v>132</v>
+      <c r="C31" s="82" t="s">
+        <v>274</v>
       </c>
       <c r="D31" s="37" t="s">
         <v>124</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F31" s="22"/>
       <c r="H31" s="22" t="s">
@@ -5523,7 +5666,7 @@
         <v>1</v>
       </c>
       <c r="N31" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O31" s="22"/>
     </row>
@@ -5632,13 +5775,13 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>133</v>
+        <v>276</v>
       </c>
       <c r="D35" s="35" t="s">
         <v>124</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F35" s="17" t="s">
         <v>62</v>
@@ -5650,11 +5793,11 @@
         <v>81</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J35" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" s="17" t="s">
         <v>44</v>
@@ -5673,17 +5816,17 @@
       <c r="B36" s="18">
         <v>120</v>
       </c>
-      <c r="C36" s="16" t="s">
-        <v>218</v>
+      <c r="C36" s="15" t="s">
+        <v>277</v>
       </c>
       <c r="D36" s="50" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E36" s="16" t="s">
         <v>99</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G36" s="14" t="s">
         <v>106</v>
@@ -5761,7 +5904,7 @@
     </row>
     <row r="39" spans="1:15" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="38" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B39" s="36"/>
       <c r="C39" s="35"/>
@@ -5820,7 +5963,7 @@
     </row>
     <row r="43" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="40" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B43" s="41"/>
       <c r="C43" s="42"/>
@@ -5950,14 +6093,14 @@
         <v>44</v>
       </c>
       <c r="J47" s="13">
-        <f t="shared" ref="J47:J52" si="7">IF(I47="Yes", 1, 0)</f>
+        <f t="shared" ref="J47:J49" si="7">IF(I47="Yes", 1, 0)</f>
         <v>1</v>
       </c>
       <c r="K47" s="13" t="s">
         <v>44</v>
       </c>
       <c r="L47" s="13">
-        <f t="shared" ref="L47:L52" si="8">IF(K47="Yes", 1, 0)</f>
+        <f t="shared" ref="L47:L49" si="8">IF(K47="Yes", 1, 0)</f>
         <v>1</v>
       </c>
       <c r="N47" s="13"/>
@@ -6038,135 +6181,6 @@
       </c>
       <c r="N49" s="13"/>
       <c r="O49" s="13"/>
-    </row>
-    <row r="50" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B50" s="11">
-        <v>0.42</v>
-      </c>
-      <c r="C50" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="D50" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="F50" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G50" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="H50" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="I50" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J50" s="13">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K50" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="L50" s="13">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="M50" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="N50" s="13"/>
-      <c r="O50" s="13"/>
-    </row>
-    <row r="51" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B51" s="11">
-        <v>0.4</v>
-      </c>
-      <c r="C51" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="D51" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="F51" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G51" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H51" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="I51" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J51" s="13">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K51" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="L51" s="13">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="N51" s="13"/>
-      <c r="O51" s="13"/>
-    </row>
-    <row r="52" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B52" s="11">
-        <v>0.38</v>
-      </c>
-      <c r="C52" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="D52" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="F52" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G52" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H52" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="I52" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J52" s="13">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K52" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="L52" s="13">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="N52" s="13"/>
-      <c r="O52" s="13"/>
     </row>
     <row r="53" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="41"/>
@@ -6415,14 +6429,14 @@
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J61" s="2">
         <f>SUM(J2:J59)</f>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K61" s="2" t="s">
         <v>109</v>
       </c>
       <c r="L61" s="2">
         <f>SUM(L2:L59)</f>
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
@@ -6430,7 +6444,7 @@
         <v>64</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
@@ -6478,8 +6492,153 @@
       <c r="N67" s="6"/>
       <c r="O67" s="6"/>
     </row>
+    <row r="69" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B69" s="81"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="N69" s="6"/>
+      <c r="O69" s="6"/>
+    </row>
+    <row r="70" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B70" s="11">
+        <v>0.42</v>
+      </c>
+      <c r="C70" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="D70" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G70" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H70" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="I70" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J70" s="13">
+        <f>IF(I70="Yes", 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K70" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L70" s="13">
+        <f>IF(K70="Yes", 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="M70" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="N70" s="13"/>
+      <c r="O70" s="13"/>
+    </row>
+    <row r="71" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B71" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="C71" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="D71" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="E71" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F71" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G71" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H71" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="I71" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J71" s="13">
+        <f>IF(I71="Yes", 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K71" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L71" s="13">
+        <f>IF(K71="Yes", 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="N71" s="13"/>
+      <c r="O71" s="13"/>
+    </row>
+    <row r="72" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B72" s="11">
+        <v>0.38</v>
+      </c>
+      <c r="C72" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="D72" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="E72" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F72" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G72" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H72" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="I72" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J72" s="13">
+        <f>IF(I72="Yes", 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K72" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L72" s="13">
+        <f>IF(K72="Yes", 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="N72" s="13"/>
+      <c r="O72" s="13"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="K63:K67 I2:I10 K55:K59 I61:I67 K33:K41 I33:I41 K45:K46 I54:I59 I15:I25 I45:I52 K2:K25 K49:K52 K27:K28 I27:I28 I30:I31 K30:K31">
+  <conditionalFormatting sqref="K63:K67 I2:I10 K55:K59 I61:I67 K33:K41 I33:I41 K45:K46 I54:I59 I15:I25 K2:K25 K27:K28 I27:I28 I30:I31 K30:K31 I45:I49 I70:I72 K49 K70:K72">
     <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -6541,25 +6700,25 @@
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -6585,7 +6744,7 @@
         <v>41.666666666666664</v>
       </c>
       <c r="I3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J3">
         <f>100*0.5/24</f>
@@ -6607,12 +6766,12 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E6" s="6" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E7" s="6">
         <v>14</v>
@@ -6627,7 +6786,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E8" s="6">
         <v>16</v>
@@ -6642,16 +6801,16 @@
     </row>
     <row r="9" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E9" s="6">
         <f>E8-E7</f>
@@ -6667,10 +6826,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C10">
         <v>21</v>
@@ -6689,10 +6848,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C11">
         <v>21</v>
@@ -6711,10 +6870,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C12">
         <v>21</v>
@@ -6733,10 +6892,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -6755,10 +6914,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -6777,10 +6936,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B15" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C15">
         <v>10</v>
@@ -6793,10 +6952,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C16">
         <v>8</v>
@@ -6809,7 +6968,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -6819,10 +6978,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B18" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C18">
         <v>5</v>
@@ -6835,10 +6994,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B19" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -6865,7 +7024,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C22">
         <f>SUM(C10:D20)</f>
@@ -6905,7 +7064,7 @@
     </row>
     <row r="25" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -6915,10 +7074,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B26" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C26">
         <v>10</v>
@@ -6931,10 +7090,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C27">
         <v>10</v>
@@ -6947,10 +7106,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B28" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C28">
         <v>10</v>
@@ -6963,10 +7122,10 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B29" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C29">
         <v>10</v>
@@ -6979,10 +7138,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B30" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C30">
         <v>7</v>
@@ -6995,10 +7154,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B31" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C31">
         <v>10</v>
@@ -7011,10 +7170,10 @@
     </row>
     <row r="32" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="46" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C32" s="46">
         <v>14</v>
@@ -7027,10 +7186,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B33" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C33">
         <v>25</v>
@@ -7043,10 +7202,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -7056,7 +7215,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C35">
         <f>SUM(C26:D33)</f>
@@ -7084,7 +7243,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C38">
         <f>SUM(C22,C35)</f>
@@ -7093,24 +7252,24 @@
     </row>
     <row r="41" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C42" s="2">
         <v>24</v>
@@ -7122,16 +7281,16 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -7169,17 +7328,17 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="78" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="B4" s="79"/>
       <c r="C4" s="79"/>
@@ -7187,7 +7346,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="80" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="B5" s="79"/>
       <c r="C5" s="79"/>
@@ -7195,7 +7354,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="80" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="B6" s="79"/>
       <c r="C6" s="79"/>
@@ -7203,7 +7362,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="80" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="B7" s="79"/>
       <c r="C7" s="79"/>
@@ -7211,7 +7370,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="80" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="B8" s="79"/>
       <c r="C8" s="79"/>
@@ -7219,7 +7378,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="80" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="B9" s="79"/>
       <c r="C9" s="79"/>
@@ -7227,7 +7386,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="80" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="B10" s="79"/>
       <c r="C10" s="79"/>
@@ -7235,7 +7394,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="80" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="B11" s="79"/>
       <c r="C11" s="79"/>
@@ -7243,7 +7402,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="80" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="B12" s="79"/>
       <c r="C12" s="79"/>
@@ -7251,7 +7410,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="80" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="B13" s="79"/>
       <c r="C13" s="79"/>
@@ -7259,7 +7418,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="80" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="B14" s="79"/>
       <c r="C14" s="79"/>
@@ -7267,7 +7426,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="80" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="B15" s="79"/>
       <c r="C15" s="79"/>
@@ -7275,7 +7434,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="80" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="B16" s="79"/>
       <c r="C16" s="79"/>
@@ -7283,7 +7442,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="80" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="B17" s="79"/>
       <c r="C17" s="79"/>
@@ -7291,7 +7450,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="80" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="B18" s="79"/>
       <c r="C18" s="79"/>
@@ -7299,7 +7458,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="80" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="B19" s="79"/>
       <c r="C19" s="79"/>

</xml_diff>